<commit_message>
Put selected syntax in separate function, fixed logic error
</commit_message>
<xml_diff>
--- a/odk-form-design-tips.xlsx
+++ b/odk-form-design-tips.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26207"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10123"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yanokwa/Documents/Work/Nafundi/Code/nafundi/odk-form-design-tips/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paul/GitHub/ODK-make-paper-survey/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32CDE70-00B0-7F4E-9ED4-4DF071A2E10D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="460" windowWidth="34840" windowHeight="23540" tabRatio="500"/>
+    <workbookView xWindow="-25600" yWindow="-1680" windowWidth="25600" windowHeight="20020" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="3" r:id="rId1"/>
     <sheet name="choices" sheetId="2" r:id="rId2"/>
     <sheet name="settings" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -26,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="564">
   <si>
     <t>form_id</t>
   </si>
@@ -1679,12 +1685,66 @@
   <si>
     <t>${a_number}+${b_number}=${a_b_total_automatic}. You said the total was ${a_b_total_manual}.
 If your total is not correct, please go back and correct your mistake.</t>
+  </si>
+  <si>
+    <t>breakfast</t>
+  </si>
+  <si>
+    <t>Bread</t>
+  </si>
+  <si>
+    <t>Fruit</t>
+  </si>
+  <si>
+    <t>Cereal</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Example select multiple</t>
+  </si>
+  <si>
+    <t>select_multiple breakfast</t>
+  </si>
+  <si>
+    <t>What did you have for breakfast?</t>
+  </si>
+  <si>
+    <t>You can select multiple if necessary</t>
+  </si>
+  <si>
+    <t>Example where the selected relevant syntax is necessary: to refer to select_multiple questions</t>
+  </si>
+  <si>
+    <t>select_multiple fruits</t>
+  </si>
+  <si>
+    <t>breakfast_fruit</t>
+  </si>
+  <si>
+    <t>selected($breakfast},'3')</t>
+  </si>
+  <si>
+    <t>fruits</t>
+  </si>
+  <si>
+    <t>What fruits did you eat?</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Banana</t>
+  </si>
+  <si>
+    <t>Kiwi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1798,6 +1858,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2065,12 +2128,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2082,7 +2145,7 @@
     <col min="5" max="5" width="36.5" style="5" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" style="5"/>
     <col min="7" max="7" width="22" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.33203125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" style="5" customWidth="1"/>
     <col min="9" max="9" width="19.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="28.5" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27.83203125" style="5" bestFit="1" customWidth="1"/>
@@ -2287,25 +2350,23 @@
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
     </row>
-    <row r="9" spans="1:12" ht="112" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>489</v>
+        <v>551</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>521</v>
+        <v>552</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>510</v>
+        <v>546</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>511</v>
+        <v>553</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>529</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>477</v>
-      </c>
+        <v>554</v>
+      </c>
+      <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2313,46 +2374,46 @@
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
     </row>
-    <row r="10" spans="1:12" ht="80" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>522</v>
+        <v>555</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>490</v>
+        <v>556</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>523</v>
+        <v>557</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>528</v>
+        <v>560</v>
       </c>
       <c r="E10" s="6"/>
-      <c r="F10" s="6" t="s">
-        <v>477</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>527</v>
-      </c>
-      <c r="H10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6" t="s">
+        <v>558</v>
+      </c>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
     </row>
-    <row r="11" spans="1:12" ht="80" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="112" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>505</v>
+        <v>489</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>491</v>
+        <v>521</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>492</v>
+        <v>510</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>524</v>
-      </c>
-      <c r="E11" s="6"/>
+        <v>511</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>529</v>
+      </c>
       <c r="F11" s="6" t="s">
         <v>477</v>
       </c>
@@ -2363,115 +2424,121 @@
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
     </row>
-    <row r="12" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>506</v>
+        <v>522</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
+      <c r="F12" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>527</v>
+      </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
-      <c r="K12" s="6" t="s">
-        <v>494</v>
-      </c>
+      <c r="K12" s="6"/>
       <c r="L12" s="6"/>
     </row>
-    <row r="13" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>495</v>
+        <v>505</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>530</v>
+        <v>492</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>539</v>
+        <v>524</v>
       </c>
       <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
+      <c r="F13" s="6" t="s">
+        <v>477</v>
+      </c>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
-      <c r="L13" s="6" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="L13" s="6"/>
+    </row>
+    <row r="14" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>533</v>
+        <v>506</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>478</v>
+        <v>493</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>543</v>
+        <v>525</v>
       </c>
       <c r="E14" s="6"/>
-      <c r="F14" s="6" t="s">
-        <v>477</v>
-      </c>
+      <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
+      <c r="K14" s="6" t="s">
+        <v>494</v>
+      </c>
       <c r="L14" s="6"/>
     </row>
-    <row r="15" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>533</v>
+        <v>495</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>478</v>
+        <v>496</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="E15" s="6"/>
-      <c r="F15" s="6" t="s">
-        <v>477</v>
-      </c>
+      <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-    </row>
-    <row r="16" spans="1:12" ht="32" x14ac:dyDescent="0.2">
-      <c r="A16" s="8"/>
+      <c r="L15" s="6" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>533</v>
+      </c>
       <c r="B16" s="6" t="s">
         <v>478</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>541</v>
+        <v>531</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
+      <c r="F16" s="6" t="s">
+        <v>477</v>
+      </c>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
@@ -2479,19 +2546,23 @@
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
     </row>
-    <row r="17" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>498</v>
+        <v>533</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>499</v>
+        <v>478</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>530</v>
-      </c>
-      <c r="D17" s="6"/>
+        <v>532</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>544</v>
+      </c>
       <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
+      <c r="F17" s="6" t="s">
+        <v>477</v>
+      </c>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
@@ -2499,41 +2570,37 @@
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
     </row>
-    <row r="18" spans="1:12" ht="48" x14ac:dyDescent="0.2">
-      <c r="A18" s="8" t="s">
-        <v>500</v>
-      </c>
+    <row r="18" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" s="8"/>
       <c r="B18" s="6" t="s">
-        <v>501</v>
+        <v>478</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>542</v>
-      </c>
-      <c r="D18" s="6"/>
+        <v>541</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>540</v>
+      </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
-      <c r="J18" s="6" t="s">
-        <v>534</v>
-      </c>
+      <c r="J18" s="6"/>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
     </row>
-    <row r="19" spans="1:12" ht="96" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>537</v>
+        <v>498</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>485</v>
+        <v>499</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>535</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>545</v>
-      </c>
+        <v>530</v>
+      </c>
+      <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
@@ -2543,14 +2610,58 @@
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
     </row>
-    <row r="20" spans="1:12" ht="96" x14ac:dyDescent="0.2">
-      <c r="B20" s="5" t="s">
+    <row r="20" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
+        <v>500</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>542</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6" t="s">
+        <v>534</v>
+      </c>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+    </row>
+    <row r="21" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
+        <v>537</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>485</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C21" s="6" t="s">
+        <v>535</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>545</v>
+      </c>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+    </row>
+    <row r="22" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+      <c r="B22" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>509</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>538</v>
       </c>
     </row>
@@ -2561,12 +2672,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D226"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D234"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2648,90 +2759,90 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
+        <v>546</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>547</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
+        <v>546</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>549</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
+        <v>546</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>548</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
+        <v>546</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>550</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
+        <v>559</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>561</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
+        <v>559</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>562</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" t="s">
-        <v>21</v>
+        <v>559</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>563</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" t="s">
-        <v>23</v>
+        <v>559</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>550</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -2739,10 +2850,10 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -2750,10 +2861,10 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -2761,10 +2872,10 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -2772,10 +2883,10 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -2783,10 +2894,10 @@
         <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -2794,10 +2905,10 @@
         <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -2805,10 +2916,10 @@
         <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -2816,10 +2927,10 @@
         <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -2827,10 +2938,10 @@
         <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -2838,10 +2949,10 @@
         <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -2849,10 +2960,10 @@
         <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -2860,10 +2971,10 @@
         <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="C26" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -2871,10 +2982,10 @@
         <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="C27" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -2882,10 +2993,10 @@
         <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="C28" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -2893,10 +3004,10 @@
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="C29" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -2904,10 +3015,10 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="C30" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -2915,10 +3026,10 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C31" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -2926,122 +3037,98 @@
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="C32" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="C33" t="s">
-        <v>63</v>
-      </c>
-      <c r="D33" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="B34" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="C34" t="s">
-        <v>65</v>
-      </c>
-      <c r="D34" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="C35" t="s">
-        <v>67</v>
-      </c>
-      <c r="D35" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="B36" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="C36" t="s">
-        <v>69</v>
-      </c>
-      <c r="D36" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="C37" t="s">
-        <v>71</v>
-      </c>
-      <c r="D37" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="B38" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="C38" t="s">
-        <v>73</v>
-      </c>
-      <c r="D38" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="C39" t="s">
-        <v>75</v>
-      </c>
-      <c r="D39" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="C40" t="s">
-        <v>77</v>
-      </c>
-      <c r="D40" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -3049,10 +3136,10 @@
         <v>61</v>
       </c>
       <c r="B41" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="C41" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="D41" t="s">
         <v>9</v>
@@ -3063,10 +3150,10 @@
         <v>61</v>
       </c>
       <c r="B42" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="C42" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="D42" t="s">
         <v>9</v>
@@ -3077,10 +3164,10 @@
         <v>61</v>
       </c>
       <c r="B43" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="C43" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="D43" t="s">
         <v>9</v>
@@ -3091,13 +3178,13 @@
         <v>61</v>
       </c>
       <c r="B44" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="C44" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="D44" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -3105,13 +3192,13 @@
         <v>61</v>
       </c>
       <c r="B45" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="C45" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="D45" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -3119,13 +3206,13 @@
         <v>61</v>
       </c>
       <c r="B46" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="C46" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="D46" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -3133,13 +3220,13 @@
         <v>61</v>
       </c>
       <c r="B47" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="C47" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="D47" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -3147,13 +3234,13 @@
         <v>61</v>
       </c>
       <c r="B48" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="C48" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="D48" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -3161,13 +3248,13 @@
         <v>61</v>
       </c>
       <c r="B49" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="C49" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="D49" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -3175,13 +3262,13 @@
         <v>61</v>
       </c>
       <c r="B50" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="C50" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="D50" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -3189,13 +3276,13 @@
         <v>61</v>
       </c>
       <c r="B51" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="C51" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="D51" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -3203,10 +3290,10 @@
         <v>61</v>
       </c>
       <c r="B52" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C52" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="D52" t="s">
         <v>11</v>
@@ -3217,10 +3304,10 @@
         <v>61</v>
       </c>
       <c r="B53" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="C53" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="D53" t="s">
         <v>11</v>
@@ -3231,10 +3318,10 @@
         <v>61</v>
       </c>
       <c r="B54" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="C54" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="D54" t="s">
         <v>11</v>
@@ -3245,10 +3332,10 @@
         <v>61</v>
       </c>
       <c r="B55" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="C55" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="D55" t="s">
         <v>11</v>
@@ -3259,10 +3346,10 @@
         <v>61</v>
       </c>
       <c r="B56" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="C56" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="D56" t="s">
         <v>11</v>
@@ -3273,10 +3360,10 @@
         <v>61</v>
       </c>
       <c r="B57" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="C57" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="D57" t="s">
         <v>11</v>
@@ -3287,10 +3374,10 @@
         <v>61</v>
       </c>
       <c r="B58" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C58" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="D58" t="s">
         <v>11</v>
@@ -3301,10 +3388,10 @@
         <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="C59" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D59" t="s">
         <v>11</v>
@@ -3315,10 +3402,10 @@
         <v>61</v>
       </c>
       <c r="B60" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="C60" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D60" t="s">
         <v>11</v>
@@ -3329,10 +3416,10 @@
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="C61" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="D61" t="s">
         <v>11</v>
@@ -3343,13 +3430,13 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="C62" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="D62" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -3357,13 +3444,13 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="C63" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="D63" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -3371,13 +3458,13 @@
         <v>61</v>
       </c>
       <c r="B64" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="C64" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="D64" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -3385,13 +3472,13 @@
         <v>61</v>
       </c>
       <c r="B65" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="C65" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="D65" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -3399,13 +3486,13 @@
         <v>61</v>
       </c>
       <c r="B66" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="C66" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="D66" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -3413,13 +3500,13 @@
         <v>61</v>
       </c>
       <c r="B67" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="C67" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="D67" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -3427,13 +3514,13 @@
         <v>61</v>
       </c>
       <c r="B68" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="C68" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="D68" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -3441,13 +3528,13 @@
         <v>61</v>
       </c>
       <c r="B69" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="C69" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="D69" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -3455,10 +3542,10 @@
         <v>61</v>
       </c>
       <c r="B70" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="C70" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="D70" t="s">
         <v>13</v>
@@ -3469,10 +3556,10 @@
         <v>61</v>
       </c>
       <c r="B71" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="C71" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="D71" t="s">
         <v>13</v>
@@ -3483,10 +3570,10 @@
         <v>61</v>
       </c>
       <c r="B72" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="C72" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="D72" t="s">
         <v>13</v>
@@ -3497,10 +3584,10 @@
         <v>61</v>
       </c>
       <c r="B73" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="C73" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="D73" t="s">
         <v>13</v>
@@ -3511,10 +3598,10 @@
         <v>61</v>
       </c>
       <c r="B74" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="C74" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="D74" t="s">
         <v>13</v>
@@ -3525,10 +3612,10 @@
         <v>61</v>
       </c>
       <c r="B75" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="C75" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="D75" t="s">
         <v>13</v>
@@ -3539,10 +3626,10 @@
         <v>61</v>
       </c>
       <c r="B76" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="C76" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="D76" t="s">
         <v>13</v>
@@ -3553,10 +3640,10 @@
         <v>61</v>
       </c>
       <c r="B77" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="C77" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="D77" t="s">
         <v>13</v>
@@ -3567,13 +3654,13 @@
         <v>61</v>
       </c>
       <c r="B78" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="C78" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="D78" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -3581,13 +3668,13 @@
         <v>61</v>
       </c>
       <c r="B79" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="C79" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="D79" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -3595,13 +3682,13 @@
         <v>61</v>
       </c>
       <c r="B80" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="C80" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="D80" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -3609,13 +3696,13 @@
         <v>61</v>
       </c>
       <c r="B81" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="C81" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="D81" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
@@ -3623,13 +3710,13 @@
         <v>61</v>
       </c>
       <c r="B82" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="C82" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="D82" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
@@ -3637,13 +3724,13 @@
         <v>61</v>
       </c>
       <c r="B83" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="C83" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="D83" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
@@ -3651,13 +3738,13 @@
         <v>61</v>
       </c>
       <c r="B84" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="C84" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="D84" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -3665,13 +3752,13 @@
         <v>61</v>
       </c>
       <c r="B85" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="C85" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="D85" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
@@ -3679,13 +3766,13 @@
         <v>61</v>
       </c>
       <c r="B86" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="C86" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="D86" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
@@ -3693,13 +3780,13 @@
         <v>61</v>
       </c>
       <c r="B87" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="C87" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="D87" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
@@ -3707,13 +3794,13 @@
         <v>61</v>
       </c>
       <c r="B88" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="C88" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="D88" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
@@ -3721,13 +3808,13 @@
         <v>61</v>
       </c>
       <c r="B89" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="C89" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="D89" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -3735,13 +3822,13 @@
         <v>61</v>
       </c>
       <c r="B90" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="C90" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="D90" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -3749,13 +3836,13 @@
         <v>61</v>
       </c>
       <c r="B91" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="C91" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="D91" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
@@ -3763,13 +3850,13 @@
         <v>61</v>
       </c>
       <c r="B92" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="C92" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="D92" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
@@ -3777,13 +3864,13 @@
         <v>61</v>
       </c>
       <c r="B93" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="C93" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="D93" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
@@ -3791,13 +3878,13 @@
         <v>61</v>
       </c>
       <c r="B94" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="C94" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="D94" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
@@ -3805,13 +3892,13 @@
         <v>61</v>
       </c>
       <c r="B95" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="C95" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="D95" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
@@ -3819,13 +3906,13 @@
         <v>61</v>
       </c>
       <c r="B96" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="C96" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="D96" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
@@ -3833,13 +3920,13 @@
         <v>61</v>
       </c>
       <c r="B97" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="C97" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
       <c r="D97" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
@@ -3847,13 +3934,13 @@
         <v>61</v>
       </c>
       <c r="B98" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="C98" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="D98" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
@@ -3861,13 +3948,13 @@
         <v>61</v>
       </c>
       <c r="B99" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
       <c r="C99" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="D99" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
@@ -3875,13 +3962,13 @@
         <v>61</v>
       </c>
       <c r="B100" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="C100" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="D100" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
@@ -3889,13 +3976,13 @@
         <v>61</v>
       </c>
       <c r="B101" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="C101" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="D101" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
@@ -3903,10 +3990,10 @@
         <v>61</v>
       </c>
       <c r="B102" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="C102" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="D102" t="s">
         <v>21</v>
@@ -3917,10 +4004,10 @@
         <v>61</v>
       </c>
       <c r="B103" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="C103" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="D103" t="s">
         <v>21</v>
@@ -3931,10 +4018,10 @@
         <v>61</v>
       </c>
       <c r="B104" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="C104" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="D104" t="s">
         <v>21</v>
@@ -3945,13 +4032,13 @@
         <v>61</v>
       </c>
       <c r="B105" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="C105" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="D105" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
@@ -3959,13 +4046,13 @@
         <v>61</v>
       </c>
       <c r="B106" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
       <c r="C106" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
       <c r="D106" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
@@ -3973,13 +4060,13 @@
         <v>61</v>
       </c>
       <c r="B107" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="C107" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="D107" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
@@ -3987,13 +4074,13 @@
         <v>61</v>
       </c>
       <c r="B108" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="C108" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="D108" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
@@ -4001,13 +4088,13 @@
         <v>61</v>
       </c>
       <c r="B109" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
       <c r="C109" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="D109" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
@@ -4015,13 +4102,13 @@
         <v>61</v>
       </c>
       <c r="B110" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="C110" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
       <c r="D110" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
@@ -4029,13 +4116,13 @@
         <v>61</v>
       </c>
       <c r="B111" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="C111" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="D111" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
@@ -4043,13 +4130,13 @@
         <v>61</v>
       </c>
       <c r="B112" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="C112" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
       <c r="D112" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
@@ -4057,13 +4144,13 @@
         <v>61</v>
       </c>
       <c r="B113" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="C113" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="D113" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
@@ -4071,13 +4158,13 @@
         <v>61</v>
       </c>
       <c r="B114" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="C114" t="s">
-        <v>225</v>
+        <v>209</v>
       </c>
       <c r="D114" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
@@ -4085,13 +4172,13 @@
         <v>61</v>
       </c>
       <c r="B115" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="C115" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="D115" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
@@ -4099,10 +4186,10 @@
         <v>61</v>
       </c>
       <c r="B116" t="s">
-        <v>228</v>
+        <v>212</v>
       </c>
       <c r="C116" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="D116" t="s">
         <v>25</v>
@@ -4113,13 +4200,13 @@
         <v>61</v>
       </c>
       <c r="B117" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="C117" t="s">
-        <v>231</v>
+        <v>215</v>
       </c>
       <c r="D117" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
@@ -4127,13 +4214,13 @@
         <v>61</v>
       </c>
       <c r="B118" t="s">
-        <v>232</v>
+        <v>216</v>
       </c>
       <c r="C118" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="D118" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
@@ -4141,13 +4228,13 @@
         <v>61</v>
       </c>
       <c r="B119" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="C119" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
       <c r="D119" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
@@ -4155,13 +4242,13 @@
         <v>61</v>
       </c>
       <c r="B120" t="s">
-        <v>236</v>
+        <v>220</v>
       </c>
       <c r="C120" t="s">
-        <v>237</v>
+        <v>221</v>
       </c>
       <c r="D120" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
@@ -4169,13 +4256,13 @@
         <v>61</v>
       </c>
       <c r="B121" t="s">
-        <v>238</v>
+        <v>222</v>
       </c>
       <c r="C121" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="D121" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
@@ -4183,13 +4270,13 @@
         <v>61</v>
       </c>
       <c r="B122" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
       <c r="C122" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="D122" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
@@ -4197,13 +4284,13 @@
         <v>61</v>
       </c>
       <c r="B123" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="C123" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="D123" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
@@ -4211,13 +4298,13 @@
         <v>61</v>
       </c>
       <c r="B124" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="C124" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
       <c r="D124" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
@@ -4225,13 +4312,13 @@
         <v>61</v>
       </c>
       <c r="B125" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="C125" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
       <c r="D125" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
@@ -4239,13 +4326,13 @@
         <v>61</v>
       </c>
       <c r="B126" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="C126" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
       <c r="D126" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
@@ -4253,13 +4340,13 @@
         <v>61</v>
       </c>
       <c r="B127" t="s">
-        <v>250</v>
+        <v>234</v>
       </c>
       <c r="C127" t="s">
-        <v>251</v>
+        <v>235</v>
       </c>
       <c r="D127" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
@@ -4267,13 +4354,13 @@
         <v>61</v>
       </c>
       <c r="B128" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="C128" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="D128" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
@@ -4281,13 +4368,13 @@
         <v>61</v>
       </c>
       <c r="B129" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
       <c r="C129" t="s">
-        <v>255</v>
+        <v>239</v>
       </c>
       <c r="D129" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
@@ -4295,13 +4382,13 @@
         <v>61</v>
       </c>
       <c r="B130" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
       <c r="C130" t="s">
-        <v>257</v>
+        <v>241</v>
       </c>
       <c r="D130" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
@@ -4309,13 +4396,13 @@
         <v>61</v>
       </c>
       <c r="B131" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="C131" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="D131" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
@@ -4323,13 +4410,13 @@
         <v>61</v>
       </c>
       <c r="B132" t="s">
-        <v>260</v>
+        <v>244</v>
       </c>
       <c r="C132" t="s">
-        <v>261</v>
+        <v>245</v>
       </c>
       <c r="D132" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
@@ -4337,10 +4424,10 @@
         <v>61</v>
       </c>
       <c r="B133" t="s">
-        <v>262</v>
+        <v>246</v>
       </c>
       <c r="C133" t="s">
-        <v>263</v>
+        <v>247</v>
       </c>
       <c r="D133" t="s">
         <v>31</v>
@@ -4351,13 +4438,13 @@
         <v>61</v>
       </c>
       <c r="B134" t="s">
-        <v>264</v>
+        <v>248</v>
       </c>
       <c r="C134" t="s">
-        <v>265</v>
+        <v>249</v>
       </c>
       <c r="D134" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
@@ -4365,13 +4452,13 @@
         <v>61</v>
       </c>
       <c r="B135" t="s">
-        <v>266</v>
+        <v>250</v>
       </c>
       <c r="C135" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
       <c r="D135" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
@@ -4379,13 +4466,13 @@
         <v>61</v>
       </c>
       <c r="B136" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
       <c r="C136" t="s">
-        <v>269</v>
+        <v>253</v>
       </c>
       <c r="D136" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
@@ -4393,13 +4480,13 @@
         <v>61</v>
       </c>
       <c r="B137" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="C137" t="s">
-        <v>271</v>
+        <v>255</v>
       </c>
       <c r="D137" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
@@ -4407,13 +4494,13 @@
         <v>61</v>
       </c>
       <c r="B138" t="s">
-        <v>272</v>
+        <v>256</v>
       </c>
       <c r="C138" t="s">
-        <v>273</v>
+        <v>257</v>
       </c>
       <c r="D138" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
@@ -4421,13 +4508,13 @@
         <v>61</v>
       </c>
       <c r="B139" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
       <c r="C139" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
       <c r="D139" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
@@ -4435,13 +4522,13 @@
         <v>61</v>
       </c>
       <c r="B140" t="s">
-        <v>276</v>
+        <v>260</v>
       </c>
       <c r="C140" t="s">
-        <v>277</v>
+        <v>261</v>
       </c>
       <c r="D140" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
@@ -4449,13 +4536,13 @@
         <v>61</v>
       </c>
       <c r="B141" t="s">
-        <v>278</v>
+        <v>262</v>
       </c>
       <c r="C141" t="s">
-        <v>279</v>
+        <v>263</v>
       </c>
       <c r="D141" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
@@ -4463,10 +4550,10 @@
         <v>61</v>
       </c>
       <c r="B142" t="s">
-        <v>280</v>
+        <v>264</v>
       </c>
       <c r="C142" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
       <c r="D142" t="s">
         <v>33</v>
@@ -4477,10 +4564,10 @@
         <v>61</v>
       </c>
       <c r="B143" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
       <c r="C143" t="s">
-        <v>283</v>
+        <v>267</v>
       </c>
       <c r="D143" t="s">
         <v>33</v>
@@ -4491,10 +4578,10 @@
         <v>61</v>
       </c>
       <c r="B144" t="s">
-        <v>284</v>
+        <v>268</v>
       </c>
       <c r="C144" t="s">
-        <v>285</v>
+        <v>269</v>
       </c>
       <c r="D144" t="s">
         <v>33</v>
@@ -4505,10 +4592,10 @@
         <v>61</v>
       </c>
       <c r="B145" t="s">
-        <v>286</v>
+        <v>270</v>
       </c>
       <c r="C145" t="s">
-        <v>287</v>
+        <v>271</v>
       </c>
       <c r="D145" t="s">
         <v>33</v>
@@ -4519,10 +4606,10 @@
         <v>61</v>
       </c>
       <c r="B146" t="s">
-        <v>288</v>
+        <v>272</v>
       </c>
       <c r="C146" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="D146" t="s">
         <v>33</v>
@@ -4533,10 +4620,10 @@
         <v>61</v>
       </c>
       <c r="B147" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="C147" t="s">
-        <v>291</v>
+        <v>275</v>
       </c>
       <c r="D147" t="s">
         <v>33</v>
@@ -4547,10 +4634,10 @@
         <v>61</v>
       </c>
       <c r="B148" t="s">
-        <v>292</v>
+        <v>276</v>
       </c>
       <c r="C148" t="s">
-        <v>293</v>
+        <v>277</v>
       </c>
       <c r="D148" t="s">
         <v>33</v>
@@ -4561,10 +4648,10 @@
         <v>61</v>
       </c>
       <c r="B149" t="s">
-        <v>294</v>
+        <v>278</v>
       </c>
       <c r="C149" t="s">
-        <v>295</v>
+        <v>279</v>
       </c>
       <c r="D149" t="s">
         <v>33</v>
@@ -4575,10 +4662,10 @@
         <v>61</v>
       </c>
       <c r="B150" t="s">
-        <v>296</v>
+        <v>280</v>
       </c>
       <c r="C150" t="s">
-        <v>297</v>
+        <v>281</v>
       </c>
       <c r="D150" t="s">
         <v>33</v>
@@ -4589,10 +4676,10 @@
         <v>61</v>
       </c>
       <c r="B151" t="s">
-        <v>298</v>
+        <v>282</v>
       </c>
       <c r="C151" t="s">
-        <v>299</v>
+        <v>283</v>
       </c>
       <c r="D151" t="s">
         <v>33</v>
@@ -4603,13 +4690,13 @@
         <v>61</v>
       </c>
       <c r="B152" t="s">
-        <v>300</v>
+        <v>284</v>
       </c>
       <c r="C152" t="s">
-        <v>301</v>
+        <v>285</v>
       </c>
       <c r="D152" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
@@ -4617,13 +4704,13 @@
         <v>61</v>
       </c>
       <c r="B153" t="s">
-        <v>302</v>
+        <v>286</v>
       </c>
       <c r="C153" t="s">
-        <v>303</v>
+        <v>287</v>
       </c>
       <c r="D153" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
@@ -4631,13 +4718,13 @@
         <v>61</v>
       </c>
       <c r="B154" t="s">
-        <v>304</v>
+        <v>288</v>
       </c>
       <c r="C154" t="s">
-        <v>305</v>
+        <v>289</v>
       </c>
       <c r="D154" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
@@ -4645,13 +4732,13 @@
         <v>61</v>
       </c>
       <c r="B155" t="s">
-        <v>306</v>
+        <v>290</v>
       </c>
       <c r="C155" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
       <c r="D155" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
@@ -4659,13 +4746,13 @@
         <v>61</v>
       </c>
       <c r="B156" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="C156" t="s">
-        <v>309</v>
+        <v>293</v>
       </c>
       <c r="D156" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
@@ -4673,13 +4760,13 @@
         <v>61</v>
       </c>
       <c r="B157" t="s">
-        <v>310</v>
+        <v>294</v>
       </c>
       <c r="C157" t="s">
-        <v>311</v>
+        <v>295</v>
       </c>
       <c r="D157" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
@@ -4687,13 +4774,13 @@
         <v>61</v>
       </c>
       <c r="B158" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
       <c r="C158" t="s">
-        <v>313</v>
+        <v>297</v>
       </c>
       <c r="D158" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
@@ -4701,13 +4788,13 @@
         <v>61</v>
       </c>
       <c r="B159" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="C159" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="D159" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
@@ -4715,10 +4802,10 @@
         <v>61</v>
       </c>
       <c r="B160" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="C160" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="D160" t="s">
         <v>35</v>
@@ -4729,10 +4816,10 @@
         <v>61</v>
       </c>
       <c r="B161" t="s">
-        <v>318</v>
+        <v>302</v>
       </c>
       <c r="C161" t="s">
-        <v>319</v>
+        <v>303</v>
       </c>
       <c r="D161" t="s">
         <v>35</v>
@@ -4743,13 +4830,13 @@
         <v>61</v>
       </c>
       <c r="B162" t="s">
-        <v>320</v>
+        <v>304</v>
       </c>
       <c r="C162" t="s">
-        <v>321</v>
+        <v>305</v>
       </c>
       <c r="D162" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
@@ -4757,13 +4844,13 @@
         <v>61</v>
       </c>
       <c r="B163" t="s">
-        <v>322</v>
+        <v>306</v>
       </c>
       <c r="C163" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
       <c r="D163" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
@@ -4771,13 +4858,13 @@
         <v>61</v>
       </c>
       <c r="B164" t="s">
-        <v>324</v>
+        <v>308</v>
       </c>
       <c r="C164" t="s">
-        <v>325</v>
+        <v>309</v>
       </c>
       <c r="D164" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
@@ -4785,13 +4872,13 @@
         <v>61</v>
       </c>
       <c r="B165" t="s">
-        <v>326</v>
+        <v>310</v>
       </c>
       <c r="C165" t="s">
-        <v>327</v>
+        <v>311</v>
       </c>
       <c r="D165" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
@@ -4799,13 +4886,13 @@
         <v>61</v>
       </c>
       <c r="B166" t="s">
-        <v>328</v>
+        <v>312</v>
       </c>
       <c r="C166" t="s">
-        <v>329</v>
+        <v>313</v>
       </c>
       <c r="D166" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
@@ -4813,13 +4900,13 @@
         <v>61</v>
       </c>
       <c r="B167" t="s">
-        <v>330</v>
+        <v>314</v>
       </c>
       <c r="C167" t="s">
-        <v>331</v>
+        <v>315</v>
       </c>
       <c r="D167" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
@@ -4827,13 +4914,13 @@
         <v>61</v>
       </c>
       <c r="B168" t="s">
-        <v>332</v>
+        <v>316</v>
       </c>
       <c r="C168" t="s">
-        <v>333</v>
+        <v>317</v>
       </c>
       <c r="D168" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
@@ -4841,13 +4928,13 @@
         <v>61</v>
       </c>
       <c r="B169" t="s">
-        <v>334</v>
+        <v>318</v>
       </c>
       <c r="C169" t="s">
-        <v>335</v>
+        <v>319</v>
       </c>
       <c r="D169" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
@@ -4855,13 +4942,13 @@
         <v>61</v>
       </c>
       <c r="B170" t="s">
-        <v>336</v>
+        <v>320</v>
       </c>
       <c r="C170" t="s">
-        <v>337</v>
+        <v>321</v>
       </c>
       <c r="D170" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
@@ -4869,10 +4956,10 @@
         <v>61</v>
       </c>
       <c r="B171" t="s">
-        <v>338</v>
+        <v>322</v>
       </c>
       <c r="C171" t="s">
-        <v>339</v>
+        <v>323</v>
       </c>
       <c r="D171" t="s">
         <v>39</v>
@@ -4883,13 +4970,13 @@
         <v>61</v>
       </c>
       <c r="B172" t="s">
-        <v>340</v>
+        <v>324</v>
       </c>
       <c r="C172" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
       <c r="D172" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
@@ -4897,13 +4984,13 @@
         <v>61</v>
       </c>
       <c r="B173" t="s">
-        <v>342</v>
+        <v>326</v>
       </c>
       <c r="C173" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
       <c r="D173" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
@@ -4911,13 +4998,13 @@
         <v>61</v>
       </c>
       <c r="B174" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C174" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
       <c r="D174" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
@@ -4925,13 +5012,13 @@
         <v>61</v>
       </c>
       <c r="B175" t="s">
-        <v>346</v>
+        <v>330</v>
       </c>
       <c r="C175" t="s">
-        <v>347</v>
+        <v>331</v>
       </c>
       <c r="D175" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
@@ -4939,13 +5026,13 @@
         <v>61</v>
       </c>
       <c r="B176" t="s">
-        <v>348</v>
+        <v>332</v>
       </c>
       <c r="C176" t="s">
-        <v>349</v>
+        <v>333</v>
       </c>
       <c r="D176" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.2">
@@ -4953,13 +5040,13 @@
         <v>61</v>
       </c>
       <c r="B177" t="s">
-        <v>350</v>
+        <v>334</v>
       </c>
       <c r="C177" t="s">
-        <v>351</v>
+        <v>335</v>
       </c>
       <c r="D177" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.2">
@@ -4967,13 +5054,13 @@
         <v>61</v>
       </c>
       <c r="B178" t="s">
-        <v>352</v>
+        <v>336</v>
       </c>
       <c r="C178" t="s">
-        <v>353</v>
+        <v>337</v>
       </c>
       <c r="D178" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.2">
@@ -4981,13 +5068,13 @@
         <v>61</v>
       </c>
       <c r="B179" t="s">
-        <v>354</v>
+        <v>338</v>
       </c>
       <c r="C179" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="D179" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.2">
@@ -4995,13 +5082,13 @@
         <v>61</v>
       </c>
       <c r="B180" t="s">
-        <v>356</v>
+        <v>340</v>
       </c>
       <c r="C180" t="s">
-        <v>357</v>
+        <v>341</v>
       </c>
       <c r="D180" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
@@ -5009,13 +5096,13 @@
         <v>61</v>
       </c>
       <c r="B181" t="s">
-        <v>358</v>
+        <v>342</v>
       </c>
       <c r="C181" t="s">
-        <v>359</v>
+        <v>343</v>
       </c>
       <c r="D181" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
@@ -5023,13 +5110,13 @@
         <v>61</v>
       </c>
       <c r="B182" t="s">
-        <v>360</v>
+        <v>344</v>
       </c>
       <c r="C182" t="s">
-        <v>361</v>
+        <v>345</v>
       </c>
       <c r="D182" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
@@ -5037,13 +5124,13 @@
         <v>61</v>
       </c>
       <c r="B183" t="s">
-        <v>362</v>
+        <v>346</v>
       </c>
       <c r="C183" t="s">
-        <v>363</v>
+        <v>347</v>
       </c>
       <c r="D183" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
@@ -5051,10 +5138,10 @@
         <v>61</v>
       </c>
       <c r="B184" t="s">
-        <v>364</v>
+        <v>348</v>
       </c>
       <c r="C184" t="s">
-        <v>365</v>
+        <v>349</v>
       </c>
       <c r="D184" t="s">
         <v>45</v>
@@ -5065,10 +5152,10 @@
         <v>61</v>
       </c>
       <c r="B185" t="s">
-        <v>366</v>
+        <v>350</v>
       </c>
       <c r="C185" t="s">
-        <v>367</v>
+        <v>351</v>
       </c>
       <c r="D185" t="s">
         <v>45</v>
@@ -5079,10 +5166,10 @@
         <v>61</v>
       </c>
       <c r="B186" t="s">
-        <v>368</v>
+        <v>352</v>
       </c>
       <c r="C186" t="s">
-        <v>369</v>
+        <v>353</v>
       </c>
       <c r="D186" t="s">
         <v>45</v>
@@ -5093,10 +5180,10 @@
         <v>61</v>
       </c>
       <c r="B187" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
       <c r="C187" t="s">
-        <v>371</v>
+        <v>355</v>
       </c>
       <c r="D187" t="s">
         <v>45</v>
@@ -5107,10 +5194,10 @@
         <v>61</v>
       </c>
       <c r="B188" t="s">
-        <v>372</v>
+        <v>356</v>
       </c>
       <c r="C188" t="s">
-        <v>373</v>
+        <v>357</v>
       </c>
       <c r="D188" t="s">
         <v>45</v>
@@ -5121,10 +5208,10 @@
         <v>61</v>
       </c>
       <c r="B189" t="s">
-        <v>374</v>
+        <v>358</v>
       </c>
       <c r="C189" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
       <c r="D189" t="s">
         <v>45</v>
@@ -5135,10 +5222,10 @@
         <v>61</v>
       </c>
       <c r="B190" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
       <c r="C190" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
       <c r="D190" t="s">
         <v>45</v>
@@ -5149,10 +5236,10 @@
         <v>61</v>
       </c>
       <c r="B191" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
       <c r="C191" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
       <c r="D191" t="s">
         <v>45</v>
@@ -5163,10 +5250,10 @@
         <v>61</v>
       </c>
       <c r="B192" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
       <c r="C192" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
       <c r="D192" t="s">
         <v>45</v>
@@ -5177,10 +5264,10 @@
         <v>61</v>
       </c>
       <c r="B193" t="s">
-        <v>382</v>
+        <v>366</v>
       </c>
       <c r="C193" t="s">
-        <v>383</v>
+        <v>367</v>
       </c>
       <c r="D193" t="s">
         <v>45</v>
@@ -5191,10 +5278,10 @@
         <v>61</v>
       </c>
       <c r="B194" t="s">
-        <v>384</v>
+        <v>368</v>
       </c>
       <c r="C194" t="s">
-        <v>385</v>
+        <v>369</v>
       </c>
       <c r="D194" t="s">
         <v>45</v>
@@ -5205,10 +5292,10 @@
         <v>61</v>
       </c>
       <c r="B195" t="s">
-        <v>386</v>
+        <v>370</v>
       </c>
       <c r="C195" t="s">
-        <v>387</v>
+        <v>371</v>
       </c>
       <c r="D195" t="s">
         <v>45</v>
@@ -5219,10 +5306,10 @@
         <v>61</v>
       </c>
       <c r="B196" t="s">
-        <v>388</v>
+        <v>372</v>
       </c>
       <c r="C196" t="s">
-        <v>389</v>
+        <v>373</v>
       </c>
       <c r="D196" t="s">
         <v>45</v>
@@ -5233,10 +5320,10 @@
         <v>61</v>
       </c>
       <c r="B197" t="s">
-        <v>390</v>
+        <v>374</v>
       </c>
       <c r="C197" t="s">
-        <v>391</v>
+        <v>375</v>
       </c>
       <c r="D197" t="s">
         <v>45</v>
@@ -5247,10 +5334,10 @@
         <v>61</v>
       </c>
       <c r="B198" t="s">
-        <v>392</v>
+        <v>376</v>
       </c>
       <c r="C198" t="s">
-        <v>393</v>
+        <v>377</v>
       </c>
       <c r="D198" t="s">
         <v>45</v>
@@ -5261,10 +5348,10 @@
         <v>61</v>
       </c>
       <c r="B199" t="s">
-        <v>394</v>
+        <v>378</v>
       </c>
       <c r="C199" t="s">
-        <v>395</v>
+        <v>379</v>
       </c>
       <c r="D199" t="s">
         <v>45</v>
@@ -5275,10 +5362,10 @@
         <v>61</v>
       </c>
       <c r="B200" t="s">
-        <v>396</v>
+        <v>380</v>
       </c>
       <c r="C200" t="s">
-        <v>397</v>
+        <v>381</v>
       </c>
       <c r="D200" t="s">
         <v>45</v>
@@ -5289,10 +5376,10 @@
         <v>61</v>
       </c>
       <c r="B201" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="C201" t="s">
-        <v>399</v>
+        <v>383</v>
       </c>
       <c r="D201" t="s">
         <v>45</v>
@@ -5303,10 +5390,10 @@
         <v>61</v>
       </c>
       <c r="B202" t="s">
-        <v>400</v>
+        <v>384</v>
       </c>
       <c r="C202" t="s">
-        <v>401</v>
+        <v>385</v>
       </c>
       <c r="D202" t="s">
         <v>45</v>
@@ -5317,13 +5404,13 @@
         <v>61</v>
       </c>
       <c r="B203" t="s">
-        <v>402</v>
+        <v>386</v>
       </c>
       <c r="C203" t="s">
-        <v>403</v>
+        <v>387</v>
       </c>
       <c r="D203" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.2">
@@ -5331,13 +5418,13 @@
         <v>61</v>
       </c>
       <c r="B204" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
       <c r="C204" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="D204" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.2">
@@ -5345,13 +5432,13 @@
         <v>61</v>
       </c>
       <c r="B205" t="s">
-        <v>406</v>
+        <v>390</v>
       </c>
       <c r="C205" t="s">
-        <v>407</v>
+        <v>391</v>
       </c>
       <c r="D205" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
@@ -5359,13 +5446,13 @@
         <v>61</v>
       </c>
       <c r="B206" t="s">
-        <v>408</v>
+        <v>392</v>
       </c>
       <c r="C206" t="s">
-        <v>409</v>
+        <v>393</v>
       </c>
       <c r="D206" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.2">
@@ -5373,13 +5460,13 @@
         <v>61</v>
       </c>
       <c r="B207" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
       <c r="C207" t="s">
-        <v>411</v>
+        <v>395</v>
       </c>
       <c r="D207" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.2">
@@ -5387,13 +5474,13 @@
         <v>61</v>
       </c>
       <c r="B208" t="s">
-        <v>412</v>
+        <v>396</v>
       </c>
       <c r="C208" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="D208" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.2">
@@ -5401,13 +5488,13 @@
         <v>61</v>
       </c>
       <c r="B209" t="s">
-        <v>414</v>
+        <v>398</v>
       </c>
       <c r="C209" t="s">
-        <v>415</v>
+        <v>399</v>
       </c>
       <c r="D209" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.2">
@@ -5415,13 +5502,13 @@
         <v>61</v>
       </c>
       <c r="B210" t="s">
-        <v>416</v>
+        <v>400</v>
       </c>
       <c r="C210" t="s">
-        <v>417</v>
+        <v>401</v>
       </c>
       <c r="D210" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.2">
@@ -5429,10 +5516,10 @@
         <v>61</v>
       </c>
       <c r="B211" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="C211" t="s">
-        <v>419</v>
+        <v>403</v>
       </c>
       <c r="D211" t="s">
         <v>47</v>
@@ -5443,10 +5530,10 @@
         <v>61</v>
       </c>
       <c r="B212" t="s">
-        <v>420</v>
+        <v>404</v>
       </c>
       <c r="C212" t="s">
-        <v>421</v>
+        <v>405</v>
       </c>
       <c r="D212" t="s">
         <v>47</v>
@@ -5457,13 +5544,13 @@
         <v>61</v>
       </c>
       <c r="B213" t="s">
-        <v>422</v>
+        <v>406</v>
       </c>
       <c r="C213" t="s">
-        <v>423</v>
+        <v>407</v>
       </c>
       <c r="D213" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.2">
@@ -5471,13 +5558,13 @@
         <v>61</v>
       </c>
       <c r="B214" t="s">
-        <v>424</v>
+        <v>408</v>
       </c>
       <c r="C214" t="s">
-        <v>425</v>
+        <v>409</v>
       </c>
       <c r="D214" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.2">
@@ -5485,13 +5572,13 @@
         <v>61</v>
       </c>
       <c r="B215" t="s">
-        <v>426</v>
+        <v>410</v>
       </c>
       <c r="C215" t="s">
-        <v>427</v>
+        <v>411</v>
       </c>
       <c r="D215" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.2">
@@ -5499,13 +5586,13 @@
         <v>61</v>
       </c>
       <c r="B216" t="s">
-        <v>428</v>
+        <v>412</v>
       </c>
       <c r="C216" t="s">
-        <v>429</v>
+        <v>413</v>
       </c>
       <c r="D216" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.2">
@@ -5513,13 +5600,13 @@
         <v>61</v>
       </c>
       <c r="B217" t="s">
-        <v>430</v>
+        <v>414</v>
       </c>
       <c r="C217" t="s">
-        <v>431</v>
+        <v>415</v>
       </c>
       <c r="D217" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.2">
@@ -5527,13 +5614,13 @@
         <v>61</v>
       </c>
       <c r="B218" t="s">
-        <v>432</v>
+        <v>416</v>
       </c>
       <c r="C218" t="s">
-        <v>433</v>
+        <v>417</v>
       </c>
       <c r="D218" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.2">
@@ -5541,13 +5628,13 @@
         <v>61</v>
       </c>
       <c r="B219" t="s">
-        <v>434</v>
+        <v>418</v>
       </c>
       <c r="C219" t="s">
-        <v>435</v>
+        <v>419</v>
       </c>
       <c r="D219" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.2">
@@ -5555,13 +5642,13 @@
         <v>61</v>
       </c>
       <c r="B220" t="s">
-        <v>436</v>
+        <v>420</v>
       </c>
       <c r="C220" t="s">
-        <v>437</v>
+        <v>421</v>
       </c>
       <c r="D220" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.2">
@@ -5569,13 +5656,13 @@
         <v>61</v>
       </c>
       <c r="B221" t="s">
-        <v>438</v>
+        <v>422</v>
       </c>
       <c r="C221" t="s">
-        <v>439</v>
+        <v>423</v>
       </c>
       <c r="D221" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.2">
@@ -5583,13 +5670,13 @@
         <v>61</v>
       </c>
       <c r="B222" t="s">
-        <v>440</v>
+        <v>424</v>
       </c>
       <c r="C222" t="s">
-        <v>441</v>
+        <v>425</v>
       </c>
       <c r="D222" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.2">
@@ -5597,13 +5684,13 @@
         <v>61</v>
       </c>
       <c r="B223" t="s">
-        <v>442</v>
+        <v>426</v>
       </c>
       <c r="C223" t="s">
-        <v>443</v>
+        <v>427</v>
       </c>
       <c r="D223" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.2">
@@ -5611,13 +5698,13 @@
         <v>61</v>
       </c>
       <c r="B224" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="C224" t="s">
-        <v>445</v>
+        <v>429</v>
       </c>
       <c r="D224" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
@@ -5625,13 +5712,13 @@
         <v>61</v>
       </c>
       <c r="B225" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="C225" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D225" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.2">
@@ -5639,12 +5726,124 @@
         <v>61</v>
       </c>
       <c r="B226" t="s">
+        <v>432</v>
+      </c>
+      <c r="C226" t="s">
+        <v>433</v>
+      </c>
+      <c r="D226" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A227" t="s">
+        <v>61</v>
+      </c>
+      <c r="B227" t="s">
+        <v>434</v>
+      </c>
+      <c r="C227" t="s">
+        <v>435</v>
+      </c>
+      <c r="D227" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A228" t="s">
+        <v>61</v>
+      </c>
+      <c r="B228" t="s">
+        <v>436</v>
+      </c>
+      <c r="C228" t="s">
+        <v>437</v>
+      </c>
+      <c r="D228" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
+        <v>61</v>
+      </c>
+      <c r="B229" t="s">
+        <v>438</v>
+      </c>
+      <c r="C229" t="s">
+        <v>439</v>
+      </c>
+      <c r="D229" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A230" t="s">
+        <v>61</v>
+      </c>
+      <c r="B230" t="s">
+        <v>440</v>
+      </c>
+      <c r="C230" t="s">
+        <v>441</v>
+      </c>
+      <c r="D230" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A231" t="s">
+        <v>61</v>
+      </c>
+      <c r="B231" t="s">
+        <v>442</v>
+      </c>
+      <c r="C231" t="s">
+        <v>443</v>
+      </c>
+      <c r="D231" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A232" t="s">
+        <v>61</v>
+      </c>
+      <c r="B232" t="s">
+        <v>444</v>
+      </c>
+      <c r="C232" t="s">
+        <v>445</v>
+      </c>
+      <c r="D232" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A233" t="s">
+        <v>61</v>
+      </c>
+      <c r="B233" t="s">
+        <v>446</v>
+      </c>
+      <c r="C233" t="s">
+        <v>447</v>
+      </c>
+      <c r="D233" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A234" t="s">
+        <v>61</v>
+      </c>
+      <c r="B234" t="s">
         <v>448</v>
       </c>
-      <c r="C226" t="s">
+      <c r="C234" t="s">
         <v>449</v>
       </c>
-      <c r="D226" t="s">
+      <c r="D234" t="s">
         <v>59</v>
       </c>
     </row>
@@ -5655,7 +5854,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>